<commit_message>
Add rows of data to Excel sheets
</commit_message>
<xml_diff>
--- a/lib/office/content/Blank.xlsx
+++ b/lib/office/content/Blank.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>